<commit_message>
Update commit for G7 killer
</commit_message>
<xml_diff>
--- a/Factures_Extraites_Multifichiers.xlsx
+++ b/Factures_Extraites_Multifichiers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TW1_033146195</t>
+          <t>TW1_033791184</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>21,20 €</t>
+          <t>20,00 €</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>TW1_033146195_004089382_00302432711.pdf</t>
+          <t>TW1_033791184_004089382_00304015690.pdf</t>
         </is>
       </c>
     </row>
@@ -511,32 +511,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TW1_033148339</t>
+          <t>TW1_033844533</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>17, Rue de Téhéran, 75008 PARIS- 8EME</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>28, Rue Petit, 92110 CLICHY</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>8, Rue Yves Du Manoir, 92420 VAUCRESSON</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>38,50 €</t>
+          <t>29,50 €</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>TW1_033148339_004089382_00302438254.pdf</t>
+          <t>TW1_033844533_004089382_00304130605.pdf</t>
         </is>
       </c>
     </row>
@@ -546,17 +546,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TW1_033201665</t>
+          <t>TW1_033856935</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>05/09/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>87, Avenue du Général Michel Bizot, 75012 PARIS-12EME</t>
+          <t>28, Rue Petit, 92110 CLICHY</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -566,12 +566,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>36,30 €</t>
+          <t>23,10 €</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TW1_033201665_004089382_00302576801.pdf</t>
+          <t>TW1_033856935_004089382_00304167026.pdf</t>
         </is>
       </c>
     </row>
@@ -581,12 +581,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TW1_033204903</t>
+          <t>TW1_033894205</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>05/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -601,12 +601,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>21,50 €</t>
+          <t>22,40 €</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>TW1_033204903_004089382_00302586283.pdf</t>
+          <t>TW1_033894205_004089382_00304261950.pdf</t>
         </is>
       </c>
     </row>
@@ -616,137 +616,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TW1_033210178</t>
+          <t>TW1_033901495</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>05/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17, Rue de Téhéran, 75008 PARIS- 8EME</t>
+          <t>28, Rue Petit, 92110 CLICHY</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>17, Rue de Téhéran, 75008 PARIS- 8EME</t>
+          <t>15, Rue Charles Duflos, 92270 BOIS-COLOMBES</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9,00 €</t>
+          <t>21,10 €</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>TW1_033210178_004089382_00302601005.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>TW1_033210922</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>05/09/2024</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>28, Rue Petit, 92110 CLICHY</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>17, Rue de Téhéran, 75008 PARIS- 8EME</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>18,00 €</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>TW1_033210922_004089382_00302601679.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TW1_033276579</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>09/09/2024</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>17, Rue de Téhéran, 75008 PARIS- 8EME</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>28, Rue Petit, 92110 CLICHY</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>22,70 €</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>TW1_033276579_004089382_00302746943.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>TW1_033280895</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>09/09/2024</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>28, Rue Petit, 92110 CLICHY</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>17, Rue de Téhéran, 75008 PARIS- 8EME</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>20,60 €</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>TW1_033280895_004089382_00302760456.pdf</t>
+          <t>TW1_033901495_004089382_00304282644.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>